<commit_message>
remove tabs related to birth order, interval and maternal age
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/subregionSpreadsheets/Barisal.xlsx
+++ b/input_spreadsheets/Bangladesh/subregionSpreadsheets/Barisal.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27224"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/discworld/Documents/Research/Health/Optima/Nutrition/development/Nutrition/input_spreadsheets/Bangladesh/subregionSpreadsheets/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-33120" yWindow="-1940" windowWidth="25600" windowHeight="16060" tabRatio="500" firstSheet="18" activeTab="19"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14100" tabRatio="500" firstSheet="22" activeTab="24"/>
   </bookViews>
   <sheets>
     <sheet name="demographics" sheetId="1" r:id="rId1"/>
@@ -32,13 +37,12 @@
     <sheet name="Interventions affected fraction" sheetId="23" r:id="rId23"/>
     <sheet name="Interventions mortality eff" sheetId="24" r:id="rId24"/>
     <sheet name="Interventions incidence eff" sheetId="25" r:id="rId25"/>
-    <sheet name="RR birth by type" sheetId="26" r:id="rId26"/>
-    <sheet name="birth distribution" sheetId="27" r:id="rId27"/>
-    <sheet name="time between births" sheetId="28" r:id="rId28"/>
-    <sheet name="RR birth by time" sheetId="29" r:id="rId29"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -263,7 +267,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="78">
   <si>
     <t>indicators</t>
   </si>
@@ -497,36 +501,6 @@
   </si>
   <si>
     <t>Interventions</t>
-  </si>
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t>&lt;18 years</t>
-  </si>
-  <si>
-    <t>18-34 years</t>
-  </si>
-  <si>
-    <t>35-49 years</t>
-  </si>
-  <si>
-    <t>first</t>
-  </si>
-  <si>
-    <t>second or third</t>
-  </si>
-  <si>
-    <t>greater than third</t>
-  </si>
-  <si>
-    <t>&lt;18 months</t>
-  </si>
-  <si>
-    <t>18-23 months</t>
-  </si>
-  <si>
-    <t>&lt;24 months</t>
   </si>
 </sst>
 </file>
@@ -817,6 +791,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1362,12 +1341,12 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="25.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" customHeight="1">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1375,7 +1354,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" customHeight="1">
+    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1383,7 +1362,7 @@
         <v>867804.96938603546</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75" customHeight="1">
+    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -1391,7 +1370,7 @@
         <v>177974.0481272742</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" customHeight="1">
+    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -1399,7 +1378,7 @@
         <v>204555.28420119709</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.75" customHeight="1">
+    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -1407,21 +1386,16 @@
         <v>0.38500000000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.75" customHeight="1">
+    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="2"/>
     </row>
-    <row r="7" spans="1:2" ht="15.75" customHeight="1">
+    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -1431,13 +1405,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="33.83203125" customWidth="1"/>
     <col min="2" max="2" width="15.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>11</v>
       </c>
@@ -1454,7 +1428,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="3" t="s">
         <v>17</v>
       </c>
@@ -1473,7 +1447,7 @@
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="3" t="s">
         <v>18</v>
       </c>
@@ -1492,7 +1466,7 @@
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="3" t="s">
         <v>19</v>
       </c>
@@ -1511,7 +1485,7 @@
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="3" t="s">
         <v>20</v>
       </c>
@@ -1530,7 +1504,7 @@
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="3" t="s">
         <v>21</v>
       </c>
@@ -1549,7 +1523,7 @@
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="3" t="s">
         <v>22</v>
       </c>
@@ -1568,7 +1542,7 @@
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1">
+    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="3" t="s">
         <v>54</v>
       </c>
@@ -1587,7 +1561,7 @@
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1">
+    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="3" t="s">
         <v>24</v>
       </c>
@@ -1606,117 +1580,112 @@
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
     </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1">
+    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
     </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1">
+    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
     </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1">
+    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
     </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1">
+    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
     </row>
-    <row r="14" spans="1:7" ht="15.75" customHeight="1">
+    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
     </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1">
+    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
     </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1">
+    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
     </row>
-    <row r="17" spans="2:7" ht="15.75" customHeight="1">
+    <row r="17" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
     </row>
-    <row r="18" spans="2:7" ht="15.75" customHeight="1">
+    <row r="18" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
     </row>
-    <row r="19" spans="2:7" ht="15.75" customHeight="1">
+    <row r="19" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
     </row>
-    <row r="20" spans="2:7" ht="15.75" customHeight="1">
+    <row r="20" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
     </row>
-    <row r="21" spans="2:7" ht="15.75" customHeight="1">
+    <row r="21" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
     </row>
-    <row r="22" spans="2:7" ht="15.75" customHeight="1">
+    <row r="22" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
     </row>
-    <row r="23" spans="2:7" ht="15.75" customHeight="1">
+    <row r="23" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
     </row>
-    <row r="24" spans="2:7" ht="15.75" customHeight="1">
+    <row r="24" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
     </row>
-    <row r="25" spans="2:7" ht="15.75" customHeight="1">
+    <row r="25" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
     </row>
-    <row r="26" spans="2:7" ht="15.75" customHeight="1">
+    <row r="26" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
     </row>
-    <row r="27" spans="2:7" ht="15.75" customHeight="1">
+    <row r="27" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
     </row>
-    <row r="28" spans="2:7" ht="15.75" customHeight="1">
+    <row r="28" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
     </row>
-    <row r="29" spans="2:7" ht="15.75" customHeight="1">
+    <row r="29" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -1728,9 +1697,9 @@
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" customHeight="1">
+    <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>13</v>
       </c>
@@ -1744,7 +1713,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.75" customHeight="1">
+    <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2">
         <v>11.2</v>
       </c>
@@ -1760,11 +1729,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -1776,9 +1740,9 @@
       <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>55</v>
       </c>
@@ -1798,7 +1762,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>25</v>
       </c>
@@ -1818,7 +1782,7 @@
         <v>2.211645569620253</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>26</v>
       </c>
@@ -1841,11 +1805,6 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -1855,12 +1814,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="25.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>56</v>
       </c>
@@ -1880,7 +1839,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>43</v>
       </c>
@@ -1900,7 +1859,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>44</v>
       </c>
@@ -1920,7 +1879,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1">
+    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
         <v>45</v>
       </c>
@@ -1940,7 +1899,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.75" customHeight="1">
+    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
         <v>46</v>
       </c>
@@ -1962,11 +1921,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -1976,9 +1930,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>55</v>
       </c>
@@ -1998,7 +1952,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>25</v>
       </c>
@@ -2020,11 +1974,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -2034,9 +1983,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" customHeight="1">
+    <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>53</v>
       </c>
@@ -2050,7 +1999,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.75" customHeight="1">
+    <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10">
         <v>1</v>
       </c>
@@ -2066,11 +2015,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -2080,12 +2024,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="43.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>57</v>
       </c>
@@ -2105,7 +2049,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>58</v>
       </c>
@@ -2125,7 +2069,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -2133,7 +2077,7 @@
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
     </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1">
+    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -2141,7 +2085,7 @@
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
     </row>
-    <row r="5" spans="1:6" ht="15.75" customHeight="1">
+    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -2151,11 +2095,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -2165,12 +2104,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="70.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>59</v>
       </c>
@@ -2190,7 +2129,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>60</v>
       </c>
@@ -2210,7 +2149,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>61</v>
       </c>
@@ -2230,7 +2169,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1">
+    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
         <v>62</v>
       </c>
@@ -2250,7 +2189,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.75" customHeight="1">
+    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
         <v>63</v>
       </c>
@@ -2272,11 +2211,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -2286,13 +2220,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="43.1640625" customWidth="1"/>
     <col min="2" max="6" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>57</v>
       </c>
@@ -2312,7 +2246,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="14">
+    <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>64</v>
       </c>
@@ -2332,7 +2266,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -2340,7 +2274,7 @@
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
     </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1">
+    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -2350,11 +2284,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -2364,12 +2293,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="5" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" customHeight="1">
+    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -2386,7 +2315,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="14">
+    <row r="2" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>43</v>
       </c>
@@ -2403,14 +2332,14 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15.75" customHeight="1">
+    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:5" ht="15.75" customHeight="1">
+    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -2419,11 +2348,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -2435,13 +2359,13 @@
       <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="12.5" customWidth="1"/>
     <col min="2" max="2" width="16.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" customHeight="1">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>6</v>
       </c>
@@ -2449,7 +2373,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" customHeight="1">
+    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5">
         <v>2017</v>
       </c>
@@ -2457,7 +2381,7 @@
         <v>176353.82451576061</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75" customHeight="1">
+    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5">
         <v>2018</v>
       </c>
@@ -2465,7 +2389,7 @@
         <v>174658.49535266697</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" customHeight="1">
+    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5">
         <v>2019</v>
       </c>
@@ -2473,7 +2397,7 @@
         <v>172874.16606401838</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.75" customHeight="1">
+    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5">
         <v>2020</v>
       </c>
@@ -2481,7 +2405,7 @@
         <v>170992.31253564314</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.75" customHeight="1">
+    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5">
         <v>2021</v>
       </c>
@@ -2489,7 +2413,7 @@
         <v>169202.0905352431</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.75" customHeight="1">
+    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="5">
         <v>2022</v>
       </c>
@@ -2497,7 +2421,7 @@
         <v>167575.14221940024</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.75" customHeight="1">
+    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="5">
         <v>2023</v>
       </c>
@@ -2505,7 +2429,7 @@
         <v>165837.38011789907</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.75" customHeight="1">
+    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="5">
         <v>2024</v>
       </c>
@@ -2513,7 +2437,7 @@
         <v>163993.39377659772</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15.75" customHeight="1">
+    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="5">
         <v>2025</v>
       </c>
@@ -2521,7 +2445,7 @@
         <v>162044.77343532885</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15.75" customHeight="1">
+    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="5">
         <v>2026</v>
       </c>
@@ -2529,7 +2453,7 @@
         <v>159507.77480490523</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="15.75" customHeight="1">
+    <row r="12" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="5">
         <v>2027</v>
       </c>
@@ -2537,7 +2461,7 @@
         <v>157416.57333469548</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="15.75" customHeight="1">
+    <row r="13" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="5">
         <v>2028</v>
       </c>
@@ -2545,7 +2469,7 @@
         <v>155245.66651214968</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="15.75" customHeight="1">
+    <row r="14" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="5">
         <v>2029</v>
       </c>
@@ -2553,7 +2477,7 @@
         <v>152997.78653795182</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="15.75" customHeight="1">
+    <row r="15" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="5">
         <v>2030</v>
       </c>
@@ -2564,11 +2488,6 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <legacyDrawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -2576,11 +2495,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="37.83203125" customWidth="1"/>
     <col min="2" max="2" width="20" customWidth="1"/>
@@ -2588,7 +2507,7 @@
     <col min="4" max="4" width="20.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>57</v>
       </c>
@@ -2602,7 +2521,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>58</v>
       </c>
@@ -2619,7 +2538,7 @@
       <c r="F2" s="13"/>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>68</v>
       </c>
@@ -2636,7 +2555,7 @@
       <c r="F3" s="13"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
         <v>69</v>
       </c>
@@ -2653,7 +2572,7 @@
       <c r="F4" s="13"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
         <v>70</v>
       </c>
@@ -2670,7 +2589,7 @@
       <c r="F5" s="13"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
         <v>64</v>
       </c>
@@ -2687,7 +2606,7 @@
       <c r="F6" s="13"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>71</v>
       </c>
@@ -2704,7 +2623,7 @@
       <c r="F7" s="13"/>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1">
+    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="3" t="s">
         <v>72</v>
       </c>
@@ -2721,110 +2640,105 @@
       <c r="F8" s="13"/>
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1">
+    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
     </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1">
+    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
     </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1">
+    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
     </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1">
+    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
     </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1">
+    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
     </row>
-    <row r="14" spans="1:7" ht="15.75" customHeight="1">
+    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
     </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1">
+    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
     </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1">
+    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
     </row>
-    <row r="17" spans="2:3" ht="15.75" customHeight="1">
+    <row r="17" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
     </row>
-    <row r="18" spans="2:3" ht="15.75" customHeight="1">
+    <row r="18" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
     </row>
-    <row r="19" spans="2:3" ht="15.75" customHeight="1">
+    <row r="19" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
     </row>
-    <row r="20" spans="2:3" ht="15.75" customHeight="1">
+    <row r="20" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
     </row>
-    <row r="21" spans="2:3" ht="15.75" customHeight="1">
+    <row r="21" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
     </row>
-    <row r="22" spans="2:3" ht="15.75" customHeight="1">
+    <row r="22" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
     </row>
-    <row r="23" spans="2:3" ht="15.75" customHeight="1">
+    <row r="23" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
     </row>
-    <row r="24" spans="2:3" ht="15.75" customHeight="1">
+    <row r="24" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
     </row>
-    <row r="25" spans="2:3" ht="15.75" customHeight="1">
+    <row r="25" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
     </row>
-    <row r="26" spans="2:3" ht="15.75" customHeight="1">
+    <row r="26" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
     </row>
-    <row r="27" spans="2:3" ht="15.75" customHeight="1">
+    <row r="27" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -2836,7 +2750,7 @@
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="37.6640625" customWidth="1"/>
     <col min="2" max="6" width="13.5" customWidth="1"/>
@@ -2846,7 +2760,7 @@
     <col min="10" max="10" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" customHeight="1">
+    <row r="1" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>57</v>
       </c>
@@ -2871,7 +2785,7 @@
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
     </row>
-    <row r="2" spans="1:10" ht="15.75" customHeight="1">
+    <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>58</v>
       </c>
@@ -2894,7 +2808,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15.75" customHeight="1">
+    <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>68</v>
       </c>
@@ -2917,7 +2831,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="15.75" customHeight="1">
+    <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
         <v>69</v>
       </c>
@@ -2940,7 +2854,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="15.75" customHeight="1">
+    <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
         <v>70</v>
       </c>
@@ -2967,7 +2881,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="15.75" customHeight="1">
+    <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
         <v>64</v>
       </c>
@@ -2990,7 +2904,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="15.75" customHeight="1">
+    <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>71</v>
       </c>
@@ -3013,7 +2927,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="15.75" customHeight="1">
+    <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="3" t="s">
         <v>72</v>
       </c>
@@ -3036,110 +2950,105 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15.75" customHeight="1">
+    <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
     </row>
-    <row r="10" spans="1:10" ht="15.75" customHeight="1">
+    <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
     </row>
-    <row r="11" spans="1:10" ht="15.75" customHeight="1">
+    <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
     </row>
-    <row r="12" spans="1:10" ht="15.75" customHeight="1">
+    <row r="12" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
     </row>
-    <row r="13" spans="1:10" ht="15.75" customHeight="1">
+    <row r="13" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
     </row>
-    <row r="14" spans="1:10" ht="15.75" customHeight="1">
+    <row r="14" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
     </row>
-    <row r="15" spans="1:10" ht="15.75" customHeight="1">
+    <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
     </row>
-    <row r="16" spans="1:10" ht="15.75" customHeight="1">
+    <row r="16" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
     </row>
-    <row r="17" spans="2:3" ht="15.75" customHeight="1">
+    <row r="17" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
     </row>
-    <row r="18" spans="2:3" ht="15.75" customHeight="1">
+    <row r="18" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
     </row>
-    <row r="19" spans="2:3" ht="15.75" customHeight="1">
+    <row r="19" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
     </row>
-    <row r="20" spans="2:3" ht="15.75" customHeight="1">
+    <row r="20" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
     </row>
-    <row r="21" spans="2:3" ht="15.75" customHeight="1">
+    <row r="21" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
     </row>
-    <row r="22" spans="2:3" ht="15.75" customHeight="1">
+    <row r="22" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
     </row>
-    <row r="23" spans="2:3" ht="15.75" customHeight="1">
+    <row r="23" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
     </row>
-    <row r="24" spans="2:3" ht="15.75" customHeight="1">
+    <row r="24" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
     </row>
-    <row r="25" spans="2:3" ht="15.75" customHeight="1">
+    <row r="25" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
     </row>
-    <row r="26" spans="2:3" ht="15.75" customHeight="1">
+    <row r="26" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
     </row>
-    <row r="27" spans="2:3" ht="15.75" customHeight="1">
+    <row r="27" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -3149,12 +3058,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="30.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>57</v>
       </c>
@@ -3174,7 +3083,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>71</v>
       </c>
@@ -3194,7 +3103,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B3" t="s">
         <v>76</v>
       </c>
@@ -3214,7 +3123,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1">
+    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>72</v>
       </c>
@@ -3234,7 +3143,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.75" customHeight="1">
+    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" t="s">
         <v>76</v>
       </c>
@@ -3253,11 +3162,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -3267,12 +3171,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="25.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>77</v>
       </c>
@@ -3295,7 +3199,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>58</v>
       </c>
@@ -3318,7 +3222,7 @@
         <v>0.253</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2"/>
       <c r="B3" s="2" t="s">
         <v>26</v>
@@ -3339,7 +3243,7 @@
         <v>0.253</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
         <v>68</v>
       </c>
@@ -3362,7 +3266,7 @@
         <v>0.41599999999999998</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" s="2" t="s">
         <v>26</v>
       </c>
@@ -3382,34 +3286,29 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
     </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
     </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1">
+    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
     </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1">
+    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -3419,12 +3318,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="25.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>77</v>
       </c>
@@ -3447,7 +3346,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>58</v>
       </c>
@@ -3470,7 +3369,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2"/>
       <c r="B3" s="2" t="s">
         <v>26</v>
@@ -3491,7 +3390,7 @@
         <v>0.51</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
         <v>68</v>
       </c>
@@ -3514,7 +3413,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" s="2" t="s">
         <v>26</v>
       </c>
@@ -3534,34 +3433,29 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
     </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
     </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1">
+    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
     </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1">
+    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -3569,14 +3463,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="23.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>77</v>
       </c>
@@ -3599,7 +3493,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>58</v>
       </c>
@@ -3622,7 +3516,7 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2"/>
       <c r="B3" s="2" t="s">
         <v>26</v>
@@ -3643,7 +3537,7 @@
         <v>0.52</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
         <v>68</v>
       </c>
@@ -3666,7 +3560,7 @@
         <v>0.62</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" s="2" t="s">
         <v>26</v>
       </c>
@@ -3686,413 +3580,29 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
     </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
     </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1">
+    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
     </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1">
+    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
-  <sheetData>
-    <row r="1" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A1" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A2" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="C2" s="2">
-        <v>3.14</v>
-      </c>
-      <c r="D2" s="2">
-        <v>1.73</v>
-      </c>
-      <c r="E2" s="2">
-        <v>1.73</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="C3" s="2">
-        <v>1.6</v>
-      </c>
-      <c r="D3" s="2">
-        <v>1</v>
-      </c>
-      <c r="E3" s="2">
-        <v>1.57</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="C4" s="2">
-        <v>1.6</v>
-      </c>
-      <c r="D4" s="2">
-        <v>1</v>
-      </c>
-      <c r="E4" s="2">
-        <v>1.57</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A5" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="C5" s="2">
-        <v>1.75</v>
-      </c>
-      <c r="D5" s="2">
-        <v>1.75</v>
-      </c>
-      <c r="E5" s="2">
-        <v>1.75</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="15.75" customHeight="1">
-      <c r="B6" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="C6" s="2">
-        <v>1.4</v>
-      </c>
-      <c r="D6" s="2">
-        <v>1</v>
-      </c>
-      <c r="E6" s="2">
-        <v>1.33</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="15.75" customHeight="1">
-      <c r="B7" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="C7" s="2">
-        <v>1.4</v>
-      </c>
-      <c r="D7" s="2">
-        <v>1</v>
-      </c>
-      <c r="E7" s="2">
-        <v>1.33</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A8" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="C8" s="2">
-        <v>1.52</v>
-      </c>
-      <c r="D8" s="2">
-        <v>1.52</v>
-      </c>
-      <c r="E8" s="2">
-        <v>1.52</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="15.75" customHeight="1">
-      <c r="B9" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="C9" s="2">
-        <v>1.2</v>
-      </c>
-      <c r="D9" s="2">
-        <v>1</v>
-      </c>
-      <c r="E9" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="15.75" customHeight="1">
-      <c r="B10" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="C10" s="2">
-        <v>1.2</v>
-      </c>
-      <c r="D10" s="2">
-        <v>1</v>
-      </c>
-      <c r="E10" s="2">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
-  <sheetData>
-    <row r="1" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A1" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="E1" s="2"/>
-    </row>
-    <row r="2" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A2" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="B2" s="2">
-        <v>5.4300000000000001E-2</v>
-      </c>
-      <c r="C2" s="2">
-        <v>0.1711</v>
-      </c>
-      <c r="D2" s="2">
-        <v>2.9999999999999997E-4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A3" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="B3" s="2">
-        <v>8.9999999999999993E-3</v>
-      </c>
-      <c r="C3" s="2">
-        <v>0.36070000000000002</v>
-      </c>
-      <c r="D3" s="2">
-        <v>8.5000000000000006E-3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A4" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="B4" s="2">
-        <v>0</v>
-      </c>
-      <c r="C4" s="2">
-        <v>0.2908</v>
-      </c>
-      <c r="D4" s="2">
-        <v>0.1048</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
-  <sheetData>
-    <row r="1" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A1" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A2" s="2">
-        <v>0.2258</v>
-      </c>
-      <c r="B2" s="2">
-        <v>7.0499999999999993E-2</v>
-      </c>
-      <c r="C2" s="2">
-        <v>0.13400000000000001</v>
-      </c>
-      <c r="D2" s="2">
-        <v>0.56979999999999997</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
-  <sheetData>
-    <row r="1" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A1" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A2" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B2" s="2">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2">
-        <v>3.03</v>
-      </c>
-      <c r="D2" s="2">
-        <v>1.77</v>
-      </c>
-      <c r="E2" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A3" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B3" s="2">
-        <v>1</v>
-      </c>
-      <c r="C3" s="2">
-        <v>1.49</v>
-      </c>
-      <c r="D3" s="2">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="E3" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A4" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B4" s="2">
-        <v>1</v>
-      </c>
-      <c r="C4" s="2">
-        <v>1.41</v>
-      </c>
-      <c r="D4" s="2">
-        <v>1.18</v>
-      </c>
-      <c r="E4" s="2">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -4104,9 +3614,9 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" customHeight="1">
+    <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="6" t="s">
         <v>8</v>
       </c>
@@ -4117,7 +3627,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="14">
+    <row r="2" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="7">
         <v>21</v>
       </c>
@@ -4133,11 +3643,6 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -4149,9 +3654,9 @@
       <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -4171,7 +3676,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -4191,7 +3696,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -4211,7 +3716,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1">
+    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -4231,7 +3736,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.75" customHeight="1">
+    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -4251,7 +3756,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15.75" customHeight="1">
+    <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -4271,7 +3776,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15.75" customHeight="1">
+    <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -4291,7 +3796,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15.75" customHeight="1">
+    <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -4311,7 +3816,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15.75" customHeight="1">
+    <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>24</v>
       </c>
@@ -4331,7 +3836,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15.75" customHeight="1">
+    <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>25</v>
       </c>
@@ -4351,7 +3856,7 @@
         <v>0.14810000000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15.75" customHeight="1">
+    <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>26</v>
       </c>
@@ -4371,7 +3876,7 @@
         <v>0.2883</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15.75" customHeight="1">
+    <row r="12" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>27</v>
       </c>
@@ -4391,7 +3896,7 @@
         <v>4.1000000000000002E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15.75" customHeight="1">
+    <row r="13" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>28</v>
       </c>
@@ -4411,7 +3916,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15.75" customHeight="1">
+    <row r="14" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>29</v>
       </c>
@@ -4431,7 +3936,7 @@
         <v>6.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15.75" customHeight="1">
+    <row r="15" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>30</v>
       </c>
@@ -4451,7 +3956,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15.75" customHeight="1">
+    <row r="16" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>31</v>
       </c>
@@ -4471,7 +3976,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="15.75" customHeight="1">
+    <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>32</v>
       </c>
@@ -4491,7 +3996,7 @@
         <v>0.14510000000000001</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="15.75" customHeight="1">
+    <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>33</v>
       </c>
@@ -4513,11 +4018,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -4529,9 +4029,9 @@
       <selection activeCell="C10" sqref="C10:G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>34</v>
       </c>
@@ -4554,7 +4054,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>36</v>
       </c>
@@ -4577,7 +4077,7 @@
         <v>19.610400980935882</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B3" s="25" t="s">
         <v>38</v>
       </c>
@@ -4597,7 +4097,7 @@
         <v>25.703446248327705</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B4" s="25" t="s">
         <v>39</v>
       </c>
@@ -4617,7 +4117,7 @@
         <v>46.200712795932716</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" s="25" t="s">
         <v>40</v>
       </c>
@@ -4637,7 +4137,7 @@
         <v>12.01235975807135</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
         <v>41</v>
       </c>
@@ -4660,7 +4160,7 @@
         <v>44.848260450963195</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="29" t="s">
         <v>38</v>
       </c>
@@ -4680,7 +4180,7 @@
         <v>35.216094484570654</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1">
+    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B8" s="29" t="s">
         <v>39</v>
       </c>
@@ -4700,7 +4200,7 @@
         <v>16.455886140643354</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1">
+    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="29" t="s">
         <v>40</v>
       </c>
@@ -4720,7 +4220,7 @@
         <v>2.6376811714603732</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1">
+    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
         <v>42</v>
       </c>
@@ -4743,7 +4243,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1">
+    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="2" t="s">
         <v>44</v>
       </c>
@@ -4763,7 +4263,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1">
+    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12" s="2" t="s">
         <v>45</v>
       </c>
@@ -4783,7 +4283,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1">
+    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B13" s="2" t="s">
         <v>46</v>
       </c>
@@ -4808,11 +4308,6 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -4822,9 +4317,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" customHeight="1">
+    <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>47</v>
       </c>
@@ -4835,7 +4330,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75" customHeight="1">
+    <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2">
         <v>3.1099999999999999E-2</v>
       </c>
@@ -4848,11 +4343,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -4862,9 +4352,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>11</v>
       </c>
@@ -4887,7 +4377,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -4910,7 +4400,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B3" s="2" t="s">
         <v>38</v>
       </c>
@@ -4930,7 +4420,7 @@
         <v>1.67</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B4" s="2" t="s">
         <v>39</v>
       </c>
@@ -4950,7 +4440,7 @@
         <v>2.38</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" s="2" t="s">
         <v>40</v>
       </c>
@@ -4970,7 +4460,7 @@
         <v>6.33</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -4993,7 +4483,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="2" t="s">
         <v>38</v>
       </c>
@@ -5013,7 +4503,7 @@
         <v>1.55</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1">
+    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B8" s="2" t="s">
         <v>39</v>
       </c>
@@ -5033,7 +4523,7 @@
         <v>2.1800000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1">
+    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="2" t="s">
         <v>40</v>
       </c>
@@ -5053,7 +4543,7 @@
         <v>6.39</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1">
+    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -5076,7 +4566,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1">
+    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="2" t="s">
         <v>38</v>
       </c>
@@ -5096,7 +4586,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1">
+    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12" s="2" t="s">
         <v>39</v>
       </c>
@@ -5116,7 +4606,7 @@
         <v>2.79</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1">
+    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B13" s="2" t="s">
         <v>40</v>
       </c>
@@ -5136,7 +4626,7 @@
         <v>6.01</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15.75" customHeight="1">
+    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>29</v>
       </c>
@@ -5159,7 +4649,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1">
+    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B15" s="2" t="s">
         <v>38</v>
       </c>
@@ -5179,7 +4669,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1">
+    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B16" s="2" t="s">
         <v>39</v>
       </c>
@@ -5199,7 +4689,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="15.75" customHeight="1">
+    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B17" s="2" t="s">
         <v>40</v>
       </c>
@@ -5219,7 +4709,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="15.75" customHeight="1">
+    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>33</v>
       </c>
@@ -5242,7 +4732,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15.75" customHeight="1">
+    <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B19" s="2" t="s">
         <v>38</v>
       </c>
@@ -5262,7 +4752,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15.75" customHeight="1">
+    <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B20" s="2" t="s">
         <v>39</v>
       </c>
@@ -5282,7 +4772,7 @@
         <v>1.86</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="15.75" customHeight="1">
+    <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B21" s="2" t="s">
         <v>40</v>
       </c>
@@ -5304,11 +4794,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -5318,9 +4803,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>11</v>
       </c>
@@ -5343,7 +4828,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -5366,7 +4851,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B3" s="2" t="s">
         <v>38</v>
       </c>
@@ -5386,7 +4871,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B4" s="2" t="s">
         <v>39</v>
       </c>
@@ -5406,7 +4891,7 @@
         <v>3.41</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" s="2" t="s">
         <v>40</v>
       </c>
@@ -5426,7 +4911,7 @@
         <v>12.33</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -5449,7 +4934,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="2" t="s">
         <v>38</v>
       </c>
@@ -5469,7 +4954,7 @@
         <v>1.92</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1">
+    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B8" s="2" t="s">
         <v>39</v>
       </c>
@@ -5489,7 +4974,7 @@
         <v>4.66</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1">
+    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="2" t="s">
         <v>40</v>
       </c>
@@ -5509,7 +4994,7 @@
         <v>9.68</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1">
+    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -5532,7 +5017,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1">
+    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="2" t="s">
         <v>38</v>
       </c>
@@ -5552,7 +5037,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1">
+    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12" s="2" t="s">
         <v>39</v>
       </c>
@@ -5572,7 +5057,7 @@
         <v>2.58</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1">
+    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B13" s="2" t="s">
         <v>40</v>
       </c>
@@ -5592,7 +5077,7 @@
         <v>9.6300000000000008</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15.75" customHeight="1">
+    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>29</v>
       </c>
@@ -5615,7 +5100,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1">
+    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B15" s="2" t="s">
         <v>38</v>
       </c>
@@ -5635,7 +5120,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1">
+    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B16" s="2" t="s">
         <v>39</v>
       </c>
@@ -5655,7 +5140,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="15.75" customHeight="1">
+    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B17" s="2" t="s">
         <v>40</v>
       </c>
@@ -5675,7 +5160,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="15.75" customHeight="1">
+    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>33</v>
       </c>
@@ -5698,7 +5183,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15.75" customHeight="1">
+    <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B19" s="2" t="s">
         <v>38</v>
       </c>
@@ -5718,7 +5203,7 @@
         <v>1.65</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15.75" customHeight="1">
+    <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B20" s="2" t="s">
         <v>39</v>
       </c>
@@ -5738,7 +5223,7 @@
         <v>2.73</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="15.75" customHeight="1">
+    <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B21" s="2" t="s">
         <v>40</v>
       </c>
@@ -5760,11 +5245,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -5774,12 +5254,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="2" width="24.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>11</v>
       </c>
@@ -5802,7 +5282,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -5825,7 +5305,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B3" s="2" t="s">
         <v>44</v>
       </c>
@@ -5845,7 +5325,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B4" s="2" t="s">
         <v>45</v>
       </c>
@@ -5865,7 +5345,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" s="2" t="s">
         <v>46</v>
       </c>
@@ -5885,7 +5365,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -5908,7 +5388,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="2" t="s">
         <v>44</v>
       </c>
@@ -5928,7 +5408,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1">
+    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B8" s="2" t="s">
         <v>45</v>
       </c>
@@ -5948,7 +5428,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1">
+    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="2" t="s">
         <v>46</v>
       </c>
@@ -5968,7 +5448,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1">
+    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -5991,7 +5471,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1">
+    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="2" t="s">
         <v>44</v>
       </c>
@@ -6011,7 +5491,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1">
+    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12" s="2" t="s">
         <v>45</v>
       </c>
@@ -6031,7 +5511,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1">
+    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B13" s="2" t="s">
         <v>46</v>
       </c>
@@ -6051,7 +5531,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15.75" customHeight="1">
+    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -6074,7 +5554,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1">
+    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B15" s="2" t="s">
         <v>44</v>
       </c>
@@ -6094,7 +5574,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1">
+    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B16" s="2" t="s">
         <v>45</v>
       </c>
@@ -6114,7 +5594,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="15.75" customHeight="1">
+    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B17" s="2" t="s">
         <v>46</v>
       </c>
@@ -6134,7 +5614,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="15.75" customHeight="1">
+    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>25</v>
       </c>
@@ -6157,7 +5637,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15.75" customHeight="1">
+    <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B19" s="2" t="s">
         <v>44</v>
       </c>
@@ -6177,7 +5657,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15.75" customHeight="1">
+    <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B20" s="2" t="s">
         <v>45</v>
       </c>
@@ -6197,7 +5677,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="15.75" customHeight="1">
+    <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B21" s="2" t="s">
         <v>46</v>
       </c>
@@ -6217,7 +5697,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="15.75" customHeight="1">
+    <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
         <v>26</v>
       </c>
@@ -6240,7 +5720,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="15.75" customHeight="1">
+    <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B23" s="2" t="s">
         <v>44</v>
       </c>
@@ -6260,7 +5740,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="15.75" customHeight="1">
+    <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B24" s="2" t="s">
         <v>45</v>
       </c>
@@ -6280,7 +5760,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="15.75" customHeight="1">
+    <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B25" s="2" t="s">
         <v>46</v>
       </c>
@@ -6300,7 +5780,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="15.75" customHeight="1">
+    <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
         <v>27</v>
       </c>
@@ -6323,7 +5803,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="15.75" customHeight="1">
+    <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B27" s="2" t="s">
         <v>44</v>
       </c>
@@ -6343,7 +5823,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="15.75" customHeight="1">
+    <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B28" s="2" t="s">
         <v>45</v>
       </c>
@@ -6363,7 +5843,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="15.75" customHeight="1">
+    <row r="29" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B29" s="2" t="s">
         <v>46</v>
       </c>
@@ -6385,10 +5865,5 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update food insecure fraction for divisions of Bangladesh
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/subregionSpreadsheets/Barisal.xlsx
+++ b/input_spreadsheets/Bangladesh/subregionSpreadsheets/Barisal.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27224"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27127"/>
   <workbookPr autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/discworld/Documents/Research/Health/Optima/Nutrition/development/Nutrition/input_spreadsheets/Bangladesh/subregionSpreadsheets/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14100" tabRatio="500" firstSheet="22" activeTab="24"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14100" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="demographics" sheetId="1" r:id="rId1"/>
@@ -38,13 +33,13 @@
     <sheet name="Interventions mortality eff" sheetId="24" r:id="rId24"/>
     <sheet name="Interventions incidence eff" sheetId="25" r:id="rId25"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
@@ -1337,16 +1332,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="25.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1354,7 +1349,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:2" ht="15.75" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1362,7 +1357,7 @@
         <v>867804.96938603546</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:2" ht="15.75" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -1370,7 +1365,7 @@
         <v>177974.0481272742</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:2" ht="15.75" customHeight="1">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -1378,24 +1373,29 @@
         <v>204555.28420119709</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:2" ht="15.75" customHeight="1">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="3">
-        <v>0.38500000000000001</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>0.35099999999999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="15.75" customHeight="1">
       <c r="A6" s="2"/>
     </row>
-    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:2" ht="15.75" customHeight="1">
       <c r="A7" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1405,13 +1405,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="33.83203125" customWidth="1"/>
     <col min="2" max="2" width="15.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>11</v>
       </c>
@@ -1428,7 +1428,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1">
       <c r="A2" s="3" t="s">
         <v>17</v>
       </c>
@@ -1447,7 +1447,7 @@
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1">
       <c r="A3" s="3" t="s">
         <v>18</v>
       </c>
@@ -1466,7 +1466,7 @@
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1">
       <c r="A4" s="3" t="s">
         <v>19</v>
       </c>
@@ -1485,7 +1485,7 @@
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1">
       <c r="A5" s="3" t="s">
         <v>20</v>
       </c>
@@ -1504,7 +1504,7 @@
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1">
       <c r="A6" s="3" t="s">
         <v>21</v>
       </c>
@@ -1523,7 +1523,7 @@
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1">
       <c r="A7" s="3" t="s">
         <v>22</v>
       </c>
@@ -1542,7 +1542,7 @@
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" ht="15.75" customHeight="1">
       <c r="A8" s="3" t="s">
         <v>54</v>
       </c>
@@ -1561,7 +1561,7 @@
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:7" ht="15.75" customHeight="1">
       <c r="A9" s="3" t="s">
         <v>24</v>
       </c>
@@ -1580,112 +1580,117 @@
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
     </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:7" ht="15.75" customHeight="1">
       <c r="B10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
     </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:7" ht="15.75" customHeight="1">
       <c r="B11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
     </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:7" ht="15.75" customHeight="1">
       <c r="B12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
     </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:7" ht="15.75" customHeight="1">
       <c r="B13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
     </row>
-    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:7" ht="15.75" customHeight="1">
       <c r="B14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
     </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:7" ht="15.75" customHeight="1">
       <c r="B15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
     </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7" ht="15.75" customHeight="1">
       <c r="B16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
     </row>
-    <row r="17" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="2:7" ht="15.75" customHeight="1">
       <c r="B17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
     </row>
-    <row r="18" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="2:7" ht="15.75" customHeight="1">
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
     </row>
-    <row r="19" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="2:7" ht="15.75" customHeight="1">
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
     </row>
-    <row r="20" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="2:7" ht="15.75" customHeight="1">
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
     </row>
-    <row r="21" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="2:7" ht="15.75" customHeight="1">
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
     </row>
-    <row r="22" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="2:7" ht="15.75" customHeight="1">
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
     </row>
-    <row r="23" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="2:7" ht="15.75" customHeight="1">
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
     </row>
-    <row r="24" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="2:7" ht="15.75" customHeight="1">
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
     </row>
-    <row r="25" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="2:7" ht="15.75" customHeight="1">
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
     </row>
-    <row r="26" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="2:7" ht="15.75" customHeight="1">
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
     </row>
-    <row r="27" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="2:7" ht="15.75" customHeight="1">
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
     </row>
-    <row r="28" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="2:7" ht="15.75" customHeight="1">
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
     </row>
-    <row r="29" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="2:7" ht="15.75" customHeight="1">
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1697,9 +1702,9 @@
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:4" ht="15.75" customHeight="1">
       <c r="A1" t="s">
         <v>13</v>
       </c>
@@ -1713,7 +1718,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:4" ht="15.75" customHeight="1">
       <c r="A2" s="2">
         <v>11.2</v>
       </c>
@@ -1729,6 +1734,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1740,9 +1750,9 @@
       <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>55</v>
       </c>
@@ -1762,7 +1772,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>25</v>
       </c>
@@ -1782,7 +1792,7 @@
         <v>2.211645569620253</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>26</v>
       </c>
@@ -1805,6 +1815,11 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1814,12 +1829,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="25.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>56</v>
       </c>
@@ -1839,7 +1854,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>43</v>
       </c>
@@ -1859,7 +1874,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>44</v>
       </c>
@@ -1879,7 +1894,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:6" ht="15.75" customHeight="1">
       <c r="A4" s="2" t="s">
         <v>45</v>
       </c>
@@ -1899,7 +1914,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:6" ht="15.75" customHeight="1">
       <c r="A5" s="2" t="s">
         <v>46</v>
       </c>
@@ -1921,6 +1936,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1930,9 +1950,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>55</v>
       </c>
@@ -1952,7 +1972,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>25</v>
       </c>
@@ -1974,6 +1994,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1983,9 +2008,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="15.75" customHeight="1">
       <c r="A1" s="9" t="s">
         <v>53</v>
       </c>
@@ -1999,7 +2024,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="15.75" customHeight="1">
       <c r="A2" s="10">
         <v>1</v>
       </c>
@@ -2015,6 +2040,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2024,12 +2054,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="43.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>57</v>
       </c>
@@ -2049,7 +2079,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>58</v>
       </c>
@@ -2069,7 +2099,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -2077,7 +2107,7 @@
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
     </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:6" ht="15.75" customHeight="1">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -2085,7 +2115,7 @@
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
     </row>
-    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:6" ht="15.75" customHeight="1">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -2095,6 +2125,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2104,12 +2139,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="70.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>59</v>
       </c>
@@ -2129,7 +2164,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>60</v>
       </c>
@@ -2149,7 +2184,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>61</v>
       </c>
@@ -2169,7 +2204,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:6" ht="15.75" customHeight="1">
       <c r="A4" s="2" t="s">
         <v>62</v>
       </c>
@@ -2189,7 +2224,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:6" ht="15.75" customHeight="1">
       <c r="A5" s="2" t="s">
         <v>63</v>
       </c>
@@ -2211,6 +2246,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2220,13 +2260,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="43.1640625" customWidth="1"/>
     <col min="2" max="6" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>57</v>
       </c>
@@ -2246,7 +2286,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="14">
       <c r="A2" s="2" t="s">
         <v>64</v>
       </c>
@@ -2266,7 +2306,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -2274,7 +2314,7 @@
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
     </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:6" ht="15.75" customHeight="1">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -2284,6 +2324,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2293,12 +2338,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="5" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" ht="15.75" customHeight="1">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -2315,7 +2360,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="14">
       <c r="A2" s="7" t="s">
         <v>43</v>
       </c>
@@ -2332,14 +2377,14 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:5" ht="15.75" customHeight="1">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:5" ht="15.75" customHeight="1">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -2348,6 +2393,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2359,13 +2409,13 @@
       <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="12.5" customWidth="1"/>
     <col min="2" max="2" width="16.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1">
       <c r="A1" s="4" t="s">
         <v>6</v>
       </c>
@@ -2373,7 +2423,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="15.75" customHeight="1">
       <c r="A2" s="5">
         <v>2017</v>
       </c>
@@ -2381,7 +2431,7 @@
         <v>176353.82451576061</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" ht="15.75" customHeight="1">
       <c r="A3" s="5">
         <v>2018</v>
       </c>
@@ -2389,7 +2439,7 @@
         <v>174658.49535266697</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" ht="15.75" customHeight="1">
       <c r="A4" s="5">
         <v>2019</v>
       </c>
@@ -2397,7 +2447,7 @@
         <v>172874.16606401838</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" ht="15.75" customHeight="1">
       <c r="A5" s="5">
         <v>2020</v>
       </c>
@@ -2405,7 +2455,7 @@
         <v>170992.31253564314</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" ht="15.75" customHeight="1">
       <c r="A6" s="5">
         <v>2021</v>
       </c>
@@ -2413,7 +2463,7 @@
         <v>169202.0905352431</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" ht="15.75" customHeight="1">
       <c r="A7" s="5">
         <v>2022</v>
       </c>
@@ -2421,7 +2471,7 @@
         <v>167575.14221940024</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" ht="15.75" customHeight="1">
       <c r="A8" s="5">
         <v>2023</v>
       </c>
@@ -2429,7 +2479,7 @@
         <v>165837.38011789907</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" ht="15.75" customHeight="1">
       <c r="A9" s="5">
         <v>2024</v>
       </c>
@@ -2437,7 +2487,7 @@
         <v>163993.39377659772</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" ht="15.75" customHeight="1">
       <c r="A10" s="5">
         <v>2025</v>
       </c>
@@ -2445,7 +2495,7 @@
         <v>162044.77343532885</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" ht="15.75" customHeight="1">
       <c r="A11" s="5">
         <v>2026</v>
       </c>
@@ -2453,7 +2503,7 @@
         <v>159507.77480490523</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" ht="15.75" customHeight="1">
       <c r="A12" s="5">
         <v>2027</v>
       </c>
@@ -2461,7 +2511,7 @@
         <v>157416.57333469548</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" ht="15.75" customHeight="1">
       <c r="A13" s="5">
         <v>2028</v>
       </c>
@@ -2469,7 +2519,7 @@
         <v>155245.66651214968</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" ht="15.75" customHeight="1">
       <c r="A14" s="5">
         <v>2029</v>
       </c>
@@ -2477,7 +2527,7 @@
         <v>152997.78653795182</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" ht="15.75" customHeight="1">
       <c r="A15" s="5">
         <v>2030</v>
       </c>
@@ -2488,6 +2538,11 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2499,7 +2554,7 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="37.83203125" customWidth="1"/>
     <col min="2" max="2" width="20" customWidth="1"/>
@@ -2507,7 +2562,7 @@
     <col min="4" max="4" width="20.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>57</v>
       </c>
@@ -2521,7 +2576,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>58</v>
       </c>
@@ -2538,7 +2593,7 @@
       <c r="F2" s="13"/>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>68</v>
       </c>
@@ -2555,7 +2610,7 @@
       <c r="F3" s="13"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1">
       <c r="A4" s="2" t="s">
         <v>69</v>
       </c>
@@ -2572,7 +2627,7 @@
       <c r="F4" s="13"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1">
       <c r="A5" s="2" t="s">
         <v>70</v>
       </c>
@@ -2589,7 +2644,7 @@
       <c r="F5" s="13"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1">
       <c r="A6" s="2" t="s">
         <v>64</v>
       </c>
@@ -2606,7 +2661,7 @@
       <c r="F6" s="13"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1">
       <c r="A7" t="s">
         <v>71</v>
       </c>
@@ -2623,7 +2678,7 @@
       <c r="F7" s="13"/>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" ht="15.75" customHeight="1">
       <c r="A8" s="3" t="s">
         <v>72</v>
       </c>
@@ -2640,105 +2695,110 @@
       <c r="F8" s="13"/>
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:7" ht="15.75" customHeight="1">
       <c r="B9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
     </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:7" ht="15.75" customHeight="1">
       <c r="B10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
     </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:7" ht="15.75" customHeight="1">
       <c r="B11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
     </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:7" ht="15.75" customHeight="1">
       <c r="B12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
     </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:7" ht="15.75" customHeight="1">
       <c r="B13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
     </row>
-    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:7" ht="15.75" customHeight="1">
       <c r="B14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
     </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:7" ht="15.75" customHeight="1">
       <c r="B15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
     </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7" ht="15.75" customHeight="1">
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
     </row>
-    <row r="17" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="2:3" ht="15.75" customHeight="1">
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
     </row>
-    <row r="18" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="2:3" ht="15.75" customHeight="1">
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
     </row>
-    <row r="19" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="2:3" ht="15.75" customHeight="1">
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
     </row>
-    <row r="20" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="2:3" ht="15.75" customHeight="1">
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
     </row>
-    <row r="21" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="2:3" ht="15.75" customHeight="1">
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
     </row>
-    <row r="22" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="2:3" ht="15.75" customHeight="1">
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
     </row>
-    <row r="23" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="2:3" ht="15.75" customHeight="1">
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
     </row>
-    <row r="24" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="2:3" ht="15.75" customHeight="1">
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
     </row>
-    <row r="25" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="2:3" ht="15.75" customHeight="1">
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
     </row>
-    <row r="26" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="2:3" ht="15.75" customHeight="1">
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
     </row>
-    <row r="27" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="2:3" ht="15.75" customHeight="1">
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2750,7 +2810,7 @@
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="37.6640625" customWidth="1"/>
     <col min="2" max="6" width="13.5" customWidth="1"/>
@@ -2760,7 +2820,7 @@
     <col min="10" max="10" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:10" ht="15.75" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>57</v>
       </c>
@@ -2785,7 +2845,7 @@
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
     </row>
-    <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:10" ht="15.75" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>58</v>
       </c>
@@ -2808,7 +2868,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:10" ht="15.75" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>68</v>
       </c>
@@ -2831,7 +2891,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:10" ht="15.75" customHeight="1">
       <c r="A4" s="2" t="s">
         <v>69</v>
       </c>
@@ -2854,7 +2914,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:10" ht="15.75" customHeight="1">
       <c r="A5" s="2" t="s">
         <v>70</v>
       </c>
@@ -2863,25 +2923,25 @@
       </c>
       <c r="C5" s="5">
         <f>demographics!$B$5</f>
-        <v>0.38500000000000001</v>
+        <v>0.35099999999999998</v>
       </c>
       <c r="D5" s="5">
         <f>demographics!$B$5</f>
-        <v>0.38500000000000001</v>
+        <v>0.35099999999999998</v>
       </c>
       <c r="E5" s="5">
         <f>demographics!$B$5</f>
-        <v>0.38500000000000001</v>
+        <v>0.35099999999999998</v>
       </c>
       <c r="F5" s="5">
         <f>demographics!$B$5</f>
-        <v>0.38500000000000001</v>
+        <v>0.35099999999999998</v>
       </c>
       <c r="G5" s="5">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:10" ht="15.75" customHeight="1">
       <c r="A6" s="2" t="s">
         <v>64</v>
       </c>
@@ -2904,7 +2964,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:10" ht="15.75" customHeight="1">
       <c r="A7" t="s">
         <v>71</v>
       </c>
@@ -2927,7 +2987,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:10" ht="15.75" customHeight="1">
       <c r="A8" s="3" t="s">
         <v>72</v>
       </c>
@@ -2950,105 +3010,110 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:10" ht="15.75" customHeight="1">
       <c r="B9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
     </row>
-    <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:10" ht="15.75" customHeight="1">
       <c r="B10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
     </row>
-    <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:10" ht="15.75" customHeight="1">
       <c r="B11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
     </row>
-    <row r="12" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:10" ht="15.75" customHeight="1">
       <c r="B12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
     </row>
-    <row r="13" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:10" ht="15.75" customHeight="1">
       <c r="B13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
     </row>
-    <row r="14" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:10" ht="15.75" customHeight="1">
       <c r="B14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
     </row>
-    <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:10" ht="15.75" customHeight="1">
       <c r="B15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
     </row>
-    <row r="16" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:10" ht="15.75" customHeight="1">
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
     </row>
-    <row r="17" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="2:3" ht="15.75" customHeight="1">
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
     </row>
-    <row r="18" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="2:3" ht="15.75" customHeight="1">
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
     </row>
-    <row r="19" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="2:3" ht="15.75" customHeight="1">
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
     </row>
-    <row r="20" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="2:3" ht="15.75" customHeight="1">
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
     </row>
-    <row r="21" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="2:3" ht="15.75" customHeight="1">
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
     </row>
-    <row r="22" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="2:3" ht="15.75" customHeight="1">
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
     </row>
-    <row r="23" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="2:3" ht="15.75" customHeight="1">
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
     </row>
-    <row r="24" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="2:3" ht="15.75" customHeight="1">
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
     </row>
-    <row r="25" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="2:3" ht="15.75" customHeight="1">
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
     </row>
-    <row r="26" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="2:3" ht="15.75" customHeight="1">
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
     </row>
-    <row r="27" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="2:3" ht="15.75" customHeight="1">
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -3058,12 +3123,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="30.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>57</v>
       </c>
@@ -3083,7 +3148,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1">
       <c r="A2" t="s">
         <v>71</v>
       </c>
@@ -3103,27 +3168,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1">
       <c r="B3" t="s">
         <v>76</v>
       </c>
       <c r="C3" s="14">
         <f>demographics!$B$5</f>
-        <v>0.38500000000000001</v>
+        <v>0.35099999999999998</v>
       </c>
       <c r="D3" s="14">
         <f>demographics!$B$5</f>
-        <v>0.38500000000000001</v>
+        <v>0.35099999999999998</v>
       </c>
       <c r="E3" s="14">
         <f>demographics!$B$5</f>
-        <v>0.38500000000000001</v>
+        <v>0.35099999999999998</v>
       </c>
       <c r="F3" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:6" ht="15.75" customHeight="1">
       <c r="A4" t="s">
         <v>72</v>
       </c>
@@ -3143,7 +3208,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:6" ht="15.75" customHeight="1">
       <c r="B5" t="s">
         <v>76</v>
       </c>
@@ -3162,6 +3227,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -3171,12 +3241,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="25.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>77</v>
       </c>
@@ -3199,7 +3269,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>58</v>
       </c>
@@ -3222,7 +3292,7 @@
         <v>0.253</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1">
       <c r="A3" s="2"/>
       <c r="B3" s="2" t="s">
         <v>26</v>
@@ -3243,7 +3313,7 @@
         <v>0.253</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1">
       <c r="A4" s="2" t="s">
         <v>68</v>
       </c>
@@ -3266,7 +3336,7 @@
         <v>0.41599999999999998</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1">
       <c r="B5" s="2" t="s">
         <v>26</v>
       </c>
@@ -3286,29 +3356,34 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1">
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
     </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
     </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" ht="15.75" customHeight="1">
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
     </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:7" ht="15.75" customHeight="1">
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -3318,12 +3393,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="25.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>77</v>
       </c>
@@ -3346,7 +3421,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>58</v>
       </c>
@@ -3369,7 +3444,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1">
       <c r="A3" s="2"/>
       <c r="B3" s="2" t="s">
         <v>26</v>
@@ -3390,7 +3465,7 @@
         <v>0.51</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1">
       <c r="A4" s="2" t="s">
         <v>68</v>
       </c>
@@ -3413,7 +3488,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1">
       <c r="B5" s="2" t="s">
         <v>26</v>
       </c>
@@ -3433,29 +3508,34 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1">
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
     </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
     </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" ht="15.75" customHeight="1">
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
     </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:7" ht="15.75" customHeight="1">
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -3463,14 +3543,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="23.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>77</v>
       </c>
@@ -3493,7 +3573,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>58</v>
       </c>
@@ -3516,7 +3596,7 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1">
       <c r="A3" s="2"/>
       <c r="B3" s="2" t="s">
         <v>26</v>
@@ -3537,7 +3617,7 @@
         <v>0.52</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1">
       <c r="A4" s="2" t="s">
         <v>68</v>
       </c>
@@ -3560,7 +3640,7 @@
         <v>0.62</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1">
       <c r="B5" s="2" t="s">
         <v>26</v>
       </c>
@@ -3580,29 +3660,34 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1">
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
     </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
     </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" ht="15.75" customHeight="1">
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
     </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:7" ht="15.75" customHeight="1">
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -3614,9 +3699,9 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:3" ht="15.75" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>8</v>
       </c>
@@ -3627,7 +3712,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="14">
       <c r="A2" s="7">
         <v>21</v>
       </c>
@@ -3643,6 +3728,11 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -3654,9 +3744,9 @@
       <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -3676,7 +3766,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -3696,7 +3786,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -3716,7 +3806,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:6" ht="15.75" customHeight="1">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -3736,7 +3826,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:6" ht="15.75" customHeight="1">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -3756,7 +3846,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:6" ht="15.75" customHeight="1">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -3776,7 +3866,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:6" ht="15.75" customHeight="1">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -3796,7 +3886,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:6" ht="15.75" customHeight="1">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -3816,7 +3906,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:6" ht="15.75" customHeight="1">
       <c r="A9" t="s">
         <v>24</v>
       </c>
@@ -3836,7 +3926,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:6" ht="15.75" customHeight="1">
       <c r="A10" t="s">
         <v>25</v>
       </c>
@@ -3856,7 +3946,7 @@
         <v>0.14810000000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:6" ht="15.75" customHeight="1">
       <c r="A11" t="s">
         <v>26</v>
       </c>
@@ -3876,7 +3966,7 @@
         <v>0.2883</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:6" ht="15.75" customHeight="1">
       <c r="A12" t="s">
         <v>27</v>
       </c>
@@ -3896,7 +3986,7 @@
         <v>4.1000000000000002E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:6" ht="15.75" customHeight="1">
       <c r="A13" t="s">
         <v>28</v>
       </c>
@@ -3916,7 +4006,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:6" ht="15.75" customHeight="1">
       <c r="A14" t="s">
         <v>29</v>
       </c>
@@ -3936,7 +4026,7 @@
         <v>6.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:6" ht="15.75" customHeight="1">
       <c r="A15" t="s">
         <v>30</v>
       </c>
@@ -3956,7 +4046,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:6" ht="15.75" customHeight="1">
       <c r="A16" t="s">
         <v>31</v>
       </c>
@@ -3976,7 +4066,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:6" ht="15.75" customHeight="1">
       <c r="A17" t="s">
         <v>32</v>
       </c>
@@ -3996,7 +4086,7 @@
         <v>0.14510000000000001</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:6" ht="15.75" customHeight="1">
       <c r="A18" t="s">
         <v>33</v>
       </c>
@@ -4018,6 +4108,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -4029,9 +4124,9 @@
       <selection activeCell="C10" sqref="C10:G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>34</v>
       </c>
@@ -4054,7 +4149,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>36</v>
       </c>
@@ -4077,7 +4172,7 @@
         <v>19.610400980935882</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1">
       <c r="B3" s="25" t="s">
         <v>38</v>
       </c>
@@ -4097,7 +4192,7 @@
         <v>25.703446248327705</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1">
       <c r="B4" s="25" t="s">
         <v>39</v>
       </c>
@@ -4117,7 +4212,7 @@
         <v>46.200712795932716</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1">
       <c r="B5" s="25" t="s">
         <v>40</v>
       </c>
@@ -4137,7 +4232,7 @@
         <v>12.01235975807135</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1">
       <c r="A6" s="2" t="s">
         <v>41</v>
       </c>
@@ -4160,7 +4255,7 @@
         <v>44.848260450963195</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1">
       <c r="B7" s="29" t="s">
         <v>38</v>
       </c>
@@ -4180,7 +4275,7 @@
         <v>35.216094484570654</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" ht="15.75" customHeight="1">
       <c r="B8" s="29" t="s">
         <v>39</v>
       </c>
@@ -4200,7 +4295,7 @@
         <v>16.455886140643354</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:7" ht="15.75" customHeight="1">
       <c r="B9" s="29" t="s">
         <v>40</v>
       </c>
@@ -4220,7 +4315,7 @@
         <v>2.6376811714603732</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:7" ht="15.75" customHeight="1">
       <c r="A10" s="2" t="s">
         <v>42</v>
       </c>
@@ -4243,7 +4338,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:7" ht="15.75" customHeight="1">
       <c r="B11" s="2" t="s">
         <v>44</v>
       </c>
@@ -4263,7 +4358,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:7" ht="15.75" customHeight="1">
       <c r="B12" s="2" t="s">
         <v>45</v>
       </c>
@@ -4283,7 +4378,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:7" ht="15.75" customHeight="1">
       <c r="B13" s="2" t="s">
         <v>46</v>
       </c>
@@ -4308,6 +4403,11 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -4317,9 +4417,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:3" ht="15.75" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>47</v>
       </c>
@@ -4330,7 +4430,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:3" ht="15.75" customHeight="1">
       <c r="A2" s="2">
         <v>3.1099999999999999E-2</v>
       </c>
@@ -4343,6 +4443,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -4352,9 +4457,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>11</v>
       </c>
@@ -4377,7 +4482,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -4400,7 +4505,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1">
       <c r="B3" s="2" t="s">
         <v>38</v>
       </c>
@@ -4420,7 +4525,7 @@
         <v>1.67</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1">
       <c r="B4" s="2" t="s">
         <v>39</v>
       </c>
@@ -4440,7 +4545,7 @@
         <v>2.38</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1">
       <c r="B5" s="2" t="s">
         <v>40</v>
       </c>
@@ -4460,7 +4565,7 @@
         <v>6.33</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -4483,7 +4588,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1">
       <c r="B7" s="2" t="s">
         <v>38</v>
       </c>
@@ -4503,7 +4608,7 @@
         <v>1.55</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" ht="15.75" customHeight="1">
       <c r="B8" s="2" t="s">
         <v>39</v>
       </c>
@@ -4523,7 +4628,7 @@
         <v>2.1800000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:7" ht="15.75" customHeight="1">
       <c r="B9" s="2" t="s">
         <v>40</v>
       </c>
@@ -4543,7 +4648,7 @@
         <v>6.39</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:7" ht="15.75" customHeight="1">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -4566,7 +4671,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:7" ht="15.75" customHeight="1">
       <c r="B11" s="2" t="s">
         <v>38</v>
       </c>
@@ -4586,7 +4691,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:7" ht="15.75" customHeight="1">
       <c r="B12" s="2" t="s">
         <v>39</v>
       </c>
@@ -4606,7 +4711,7 @@
         <v>2.79</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:7" ht="15.75" customHeight="1">
       <c r="B13" s="2" t="s">
         <v>40</v>
       </c>
@@ -4626,7 +4731,7 @@
         <v>6.01</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:7" ht="15.75" customHeight="1">
       <c r="A14" t="s">
         <v>29</v>
       </c>
@@ -4649,7 +4754,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:7" ht="15.75" customHeight="1">
       <c r="B15" s="2" t="s">
         <v>38</v>
       </c>
@@ -4669,7 +4774,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7" ht="15.75" customHeight="1">
       <c r="B16" s="2" t="s">
         <v>39</v>
       </c>
@@ -4689,7 +4794,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:7" ht="15.75" customHeight="1">
       <c r="B17" s="2" t="s">
         <v>40</v>
       </c>
@@ -4709,7 +4814,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:7" ht="15.75" customHeight="1">
       <c r="A18" t="s">
         <v>33</v>
       </c>
@@ -4732,7 +4837,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:7" ht="15.75" customHeight="1">
       <c r="B19" s="2" t="s">
         <v>38</v>
       </c>
@@ -4752,7 +4857,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:7" ht="15.75" customHeight="1">
       <c r="B20" s="2" t="s">
         <v>39</v>
       </c>
@@ -4772,7 +4877,7 @@
         <v>1.86</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:7" ht="15.75" customHeight="1">
       <c r="B21" s="2" t="s">
         <v>40</v>
       </c>
@@ -4794,6 +4899,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -4803,9 +4913,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>11</v>
       </c>
@@ -4828,7 +4938,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -4851,7 +4961,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1">
       <c r="B3" s="2" t="s">
         <v>38</v>
       </c>
@@ -4871,7 +4981,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1">
       <c r="B4" s="2" t="s">
         <v>39</v>
       </c>
@@ -4891,7 +5001,7 @@
         <v>3.41</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1">
       <c r="B5" s="2" t="s">
         <v>40</v>
       </c>
@@ -4911,7 +5021,7 @@
         <v>12.33</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -4934,7 +5044,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1">
       <c r="B7" s="2" t="s">
         <v>38</v>
       </c>
@@ -4954,7 +5064,7 @@
         <v>1.92</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" ht="15.75" customHeight="1">
       <c r="B8" s="2" t="s">
         <v>39</v>
       </c>
@@ -4974,7 +5084,7 @@
         <v>4.66</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:7" ht="15.75" customHeight="1">
       <c r="B9" s="2" t="s">
         <v>40</v>
       </c>
@@ -4994,7 +5104,7 @@
         <v>9.68</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:7" ht="15.75" customHeight="1">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -5017,7 +5127,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:7" ht="15.75" customHeight="1">
       <c r="B11" s="2" t="s">
         <v>38</v>
       </c>
@@ -5037,7 +5147,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:7" ht="15.75" customHeight="1">
       <c r="B12" s="2" t="s">
         <v>39</v>
       </c>
@@ -5057,7 +5167,7 @@
         <v>2.58</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:7" ht="15.75" customHeight="1">
       <c r="B13" s="2" t="s">
         <v>40</v>
       </c>
@@ -5077,7 +5187,7 @@
         <v>9.6300000000000008</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:7" ht="15.75" customHeight="1">
       <c r="A14" t="s">
         <v>29</v>
       </c>
@@ -5100,7 +5210,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:7" ht="15.75" customHeight="1">
       <c r="B15" s="2" t="s">
         <v>38</v>
       </c>
@@ -5120,7 +5230,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7" ht="15.75" customHeight="1">
       <c r="B16" s="2" t="s">
         <v>39</v>
       </c>
@@ -5140,7 +5250,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:7" ht="15.75" customHeight="1">
       <c r="B17" s="2" t="s">
         <v>40</v>
       </c>
@@ -5160,7 +5270,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:7" ht="15.75" customHeight="1">
       <c r="A18" t="s">
         <v>33</v>
       </c>
@@ -5183,7 +5293,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:7" ht="15.75" customHeight="1">
       <c r="B19" s="2" t="s">
         <v>38</v>
       </c>
@@ -5203,7 +5313,7 @@
         <v>1.65</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:7" ht="15.75" customHeight="1">
       <c r="B20" s="2" t="s">
         <v>39</v>
       </c>
@@ -5223,7 +5333,7 @@
         <v>2.73</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:7" ht="15.75" customHeight="1">
       <c r="B21" s="2" t="s">
         <v>40</v>
       </c>
@@ -5245,6 +5355,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -5254,12 +5369,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="2" width="24.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>11</v>
       </c>
@@ -5282,7 +5397,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -5305,7 +5420,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1">
       <c r="B3" s="2" t="s">
         <v>44</v>
       </c>
@@ -5325,7 +5440,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1">
       <c r="B4" s="2" t="s">
         <v>45</v>
       </c>
@@ -5345,7 +5460,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1">
       <c r="B5" s="2" t="s">
         <v>46</v>
       </c>
@@ -5365,7 +5480,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -5388,7 +5503,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1">
       <c r="B7" s="2" t="s">
         <v>44</v>
       </c>
@@ -5408,7 +5523,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" ht="15.75" customHeight="1">
       <c r="B8" s="2" t="s">
         <v>45</v>
       </c>
@@ -5428,7 +5543,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:7" ht="15.75" customHeight="1">
       <c r="B9" s="2" t="s">
         <v>46</v>
       </c>
@@ -5448,7 +5563,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:7" ht="15.75" customHeight="1">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -5471,7 +5586,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:7" ht="15.75" customHeight="1">
       <c r="B11" s="2" t="s">
         <v>44</v>
       </c>
@@ -5491,7 +5606,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:7" ht="15.75" customHeight="1">
       <c r="B12" s="2" t="s">
         <v>45</v>
       </c>
@@ -5511,7 +5626,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:7" ht="15.75" customHeight="1">
       <c r="B13" s="2" t="s">
         <v>46</v>
       </c>
@@ -5531,7 +5646,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:7" ht="15.75" customHeight="1">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -5554,7 +5669,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:7" ht="15.75" customHeight="1">
       <c r="B15" s="2" t="s">
         <v>44</v>
       </c>
@@ -5574,7 +5689,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7" ht="15.75" customHeight="1">
       <c r="B16" s="2" t="s">
         <v>45</v>
       </c>
@@ -5594,7 +5709,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:7" ht="15.75" customHeight="1">
       <c r="B17" s="2" t="s">
         <v>46</v>
       </c>
@@ -5614,7 +5729,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:7" ht="15.75" customHeight="1">
       <c r="A18" t="s">
         <v>25</v>
       </c>
@@ -5637,7 +5752,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:7" ht="15.75" customHeight="1">
       <c r="B19" s="2" t="s">
         <v>44</v>
       </c>
@@ -5657,7 +5772,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:7" ht="15.75" customHeight="1">
       <c r="B20" s="2" t="s">
         <v>45</v>
       </c>
@@ -5677,7 +5792,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:7" ht="15.75" customHeight="1">
       <c r="B21" s="2" t="s">
         <v>46</v>
       </c>
@@ -5697,7 +5812,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:7" ht="15.75" customHeight="1">
       <c r="A22" t="s">
         <v>26</v>
       </c>
@@ -5720,7 +5835,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:7" ht="15.75" customHeight="1">
       <c r="B23" s="2" t="s">
         <v>44</v>
       </c>
@@ -5740,7 +5855,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:7" ht="15.75" customHeight="1">
       <c r="B24" s="2" t="s">
         <v>45</v>
       </c>
@@ -5760,7 +5875,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:7" ht="15.75" customHeight="1">
       <c r="B25" s="2" t="s">
         <v>46</v>
       </c>
@@ -5780,7 +5895,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:7" ht="15.75" customHeight="1">
       <c r="A26" t="s">
         <v>27</v>
       </c>
@@ -5803,7 +5918,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:7" ht="15.75" customHeight="1">
       <c r="B27" s="2" t="s">
         <v>44</v>
       </c>
@@ -5823,7 +5938,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:7" ht="15.75" customHeight="1">
       <c r="B28" s="2" t="s">
         <v>45</v>
       </c>
@@ -5843,7 +5958,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:7" ht="15.75" customHeight="1">
       <c r="B29" s="2" t="s">
         <v>46</v>
       </c>
@@ -5865,5 +5980,10 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>